<commit_message>
Updating Sprint 2 Backlog (Day 3)
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
@@ -5,10 +5,10 @@
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\OneDrive\Documents\University\Third Year\Agile\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF512612-2B0A-4972-9B7A-A5232494F642}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="1" documentId="8_{586F1A4F-9DD0-416D-B961-7BC431B036C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D69ED37E-E183-43A0-B7D9-127C9407EB8D}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -100,9 +100,6 @@
     <t xml:space="preserve">As a user, I want to use my current location, to help me locate the nearest institution. </t>
   </si>
   <si>
-    <t>Oskar</t>
-  </si>
-  <si>
     <t>Design front-end</t>
   </si>
   <si>
@@ -110,6 +107,9 @@
   </si>
   <si>
     <t>Back-end implementation</t>
+  </si>
+  <si>
+    <t>Oskar, Yousaf, Blazej and Roman</t>
   </si>
   <si>
     <t>Not Started</t>
@@ -136,9 +136,6 @@
     <t>Blazej</t>
   </si>
   <si>
-    <t>Oskar, Yousaf, Blazej and Roman</t>
-  </si>
-  <si>
     <t>As a user, I want to be able to see the price information for each result on the map, to help me make a decision on a medical institution</t>
   </si>
   <si>
@@ -155,6 +152,9 @@
   </si>
   <si>
     <t>As a user I want to search by location, to help me locate nearby institutions</t>
+  </si>
+  <si>
+    <t>Oskar</t>
   </si>
   <si>
     <t>As a user, I want to order the search results by distance, to help me identify the nearest institution for my treatment</t>
@@ -179,7 +179,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -220,13 +220,6 @@
       <color theme="0" tint="-0.499984740745262"/>
       <name val="Century Gothic"/>
       <family val="1"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -301,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -338,14 +331,13 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -471,7 +463,7 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>43.5</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>0</c:v>
@@ -594,15 +586,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>104775</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>247650</xdr:rowOff>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>47625</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>476250</xdr:colOff>
-      <xdr:row>39</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:colOff>695325</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>238125</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -960,9 +952,9 @@
   </sheetPr>
   <dimension ref="A1:AC144"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D12" sqref="D12"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -983,30 +975,30 @@
     <col min="24" max="16384" width="10.83203125" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" ht="50.15" customHeight="1" x14ac:dyDescent="0.65">
+    <row r="1" spans="1:29" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="19"/>
-      <c r="D1" s="19"/>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="19"/>
-      <c r="I1" s="19"/>
-      <c r="J1" s="19"/>
-      <c r="K1" s="19"/>
-      <c r="L1" s="19"/>
-      <c r="M1" s="19"/>
-      <c r="N1" s="19"/>
-      <c r="O1" s="19"/>
-      <c r="P1" s="19"/>
-      <c r="Q1" s="19"/>
-      <c r="R1" s="19"/>
-      <c r="S1" s="19"/>
-      <c r="T1" s="19"/>
-      <c r="U1" s="19"/>
-      <c r="V1" s="19"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+      <c r="F1" s="18"/>
+      <c r="G1" s="18"/>
+      <c r="H1" s="18"/>
+      <c r="I1" s="18"/>
+      <c r="J1" s="18"/>
+      <c r="K1" s="18"/>
+      <c r="L1" s="18"/>
+      <c r="M1" s="18"/>
+      <c r="N1" s="18"/>
+      <c r="O1" s="18"/>
+      <c r="P1" s="18"/>
+      <c r="Q1" s="18"/>
+      <c r="R1" s="18"/>
+      <c r="S1" s="18"/>
+      <c r="T1" s="18"/>
+      <c r="U1" s="18"/>
+      <c r="V1" s="18"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
@@ -1087,9 +1079,11 @@
       <c r="H3" s="7">
         <v>1</v>
       </c>
-      <c r="I3" s="8"/>
-      <c r="J3" s="8"/>
-      <c r="K3" s="8"/>
+      <c r="I3" s="7">
+        <v>0</v>
+      </c>
+      <c r="J3" s="7"/>
+      <c r="K3" s="7"/>
       <c r="L3" s="8"/>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
@@ -1160,9 +1154,11 @@
       <c r="H5" s="7">
         <v>0</v>
       </c>
-      <c r="I5" s="8"/>
-      <c r="J5" s="8"/>
-      <c r="K5" s="8"/>
+      <c r="I5" s="7">
+        <v>0</v>
+      </c>
+      <c r="J5" s="7"/>
+      <c r="K5" s="7"/>
       <c r="L5" s="8"/>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
@@ -1233,9 +1229,11 @@
       <c r="H7" s="7">
         <v>4</v>
       </c>
-      <c r="I7" s="8"/>
-      <c r="J7" s="8"/>
-      <c r="K7" s="8"/>
+      <c r="I7" s="7">
+        <v>0</v>
+      </c>
+      <c r="J7" s="7"/>
+      <c r="K7" s="7"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
@@ -1291,7 +1289,7 @@
         <v>5</v>
       </c>
       <c r="D9" s="12" t="s">
-        <v>21</v>
+        <v>16</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>19</v>
@@ -1305,9 +1303,11 @@
       <c r="H9" s="7">
         <v>4</v>
       </c>
-      <c r="I9" s="8"/>
-      <c r="J9" s="8"/>
-      <c r="K9" s="8"/>
+      <c r="I9" s="7">
+        <v>4</v>
+      </c>
+      <c r="J9" s="7"/>
+      <c r="K9" s="7"/>
       <c r="L9" s="8"/>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
@@ -1328,13 +1328,13 @@
     </row>
     <row r="10" spans="1:29" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="9" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" s="9">
+        <v>1</v>
+      </c>
+      <c r="D10" s="9" t="s">
         <v>22</v>
-      </c>
-      <c r="C10" s="9">
-        <v>1</v>
-      </c>
-      <c r="D10" s="9" t="s">
-        <v>23</v>
       </c>
       <c r="E10" s="9" t="s">
         <v>19</v>
@@ -1348,7 +1348,9 @@
       <c r="H10" s="9">
         <v>0</v>
       </c>
-      <c r="I10" s="9"/>
+      <c r="I10" s="9">
+        <v>0</v>
+      </c>
       <c r="J10" s="9"/>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
@@ -1371,13 +1373,13 @@
     </row>
     <row r="11" spans="1:29" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B11" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C11" s="9">
         <v>3</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
         <v>25</v>
@@ -1391,7 +1393,9 @@
       <c r="H11" s="9">
         <v>3</v>
       </c>
-      <c r="I11" s="9"/>
+      <c r="I11" s="9">
+        <v>3</v>
+      </c>
       <c r="J11" s="9"/>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
@@ -1434,7 +1438,9 @@
       <c r="H12" s="9">
         <v>1</v>
       </c>
-      <c r="I12" s="9"/>
+      <c r="I12" s="9">
+        <v>1</v>
+      </c>
       <c r="J12" s="9"/>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
@@ -1475,9 +1481,11 @@
       <c r="H13" s="7">
         <v>5</v>
       </c>
-      <c r="I13" s="8"/>
-      <c r="J13" s="8"/>
-      <c r="K13" s="8"/>
+      <c r="I13" s="7">
+        <v>4</v>
+      </c>
+      <c r="J13" s="7"/>
+      <c r="K13" s="7"/>
       <c r="L13" s="8"/>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
@@ -1496,7 +1504,7 @@
       <c r="AA13" s="4"/>
       <c r="AB13" s="4"/>
     </row>
-    <row r="14" spans="1:29" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:29" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="9" t="s">
         <v>30</v>
       </c>
@@ -1504,7 +1512,7 @@
         <v>2</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E14" s="9" t="s">
         <v>19</v>
@@ -1518,37 +1526,39 @@
       <c r="H14" s="9">
         <v>1</v>
       </c>
-      <c r="I14" s="9"/>
+      <c r="I14" s="9">
+        <v>0</v>
+      </c>
       <c r="J14" s="9"/>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
-      <c r="N14" s="4"/>
-      <c r="O14" s="4"/>
-      <c r="P14" s="4"/>
-      <c r="Q14" s="4"/>
-      <c r="R14" s="4"/>
-      <c r="S14" s="4"/>
-      <c r="T14" s="4"/>
-      <c r="U14" s="4"/>
-      <c r="V14" s="4"/>
-      <c r="W14" s="4"/>
-      <c r="X14" s="4"/>
-      <c r="Y14" s="4"/>
-      <c r="Z14" s="4"/>
-      <c r="AA14" s="4"/>
-      <c r="AB14" s="4"/>
-      <c r="AC14" s="4"/>
+      <c r="N14" s="11"/>
+      <c r="O14" s="11"/>
+      <c r="P14" s="11"/>
+      <c r="Q14" s="11"/>
+      <c r="R14" s="11"/>
+      <c r="S14" s="11"/>
+      <c r="T14" s="11"/>
+      <c r="U14" s="11"/>
+      <c r="V14" s="11"/>
+      <c r="W14" s="11"/>
+      <c r="X14" s="11"/>
+      <c r="Y14" s="11"/>
+      <c r="Z14" s="11"/>
+      <c r="AA14" s="11"/>
+      <c r="AB14" s="11"/>
+      <c r="AC14" s="11"/>
     </row>
     <row r="15" spans="1:29" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C15" s="9">
         <v>3</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E15" s="9" t="s">
         <v>25</v>
@@ -1562,7 +1572,9 @@
       <c r="H15" s="9">
         <v>3</v>
       </c>
-      <c r="I15" s="9"/>
+      <c r="I15" s="9">
+        <v>3</v>
+      </c>
       <c r="J15" s="9"/>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
@@ -1606,7 +1618,9 @@
       <c r="H16" s="9">
         <v>1</v>
       </c>
-      <c r="I16" s="9"/>
+      <c r="I16" s="9">
+        <v>1</v>
+      </c>
       <c r="J16" s="9"/>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
@@ -1647,9 +1661,11 @@
       <c r="H17" s="7">
         <v>5</v>
       </c>
-      <c r="I17" s="8"/>
-      <c r="J17" s="8"/>
-      <c r="K17" s="8"/>
+      <c r="I17" s="7">
+        <v>5</v>
+      </c>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
       <c r="L17" s="8"/>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
@@ -1670,13 +1686,13 @@
     </row>
     <row r="18" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C18" s="9">
         <v>3</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E18" s="9" t="s">
         <v>25</v>
@@ -1690,7 +1706,9 @@
       <c r="H18" s="9">
         <v>3</v>
       </c>
-      <c r="I18" s="9"/>
+      <c r="I18" s="9">
+        <v>3</v>
+      </c>
       <c r="J18" s="9"/>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
@@ -1733,7 +1751,9 @@
       <c r="H19" s="9">
         <v>2</v>
       </c>
-      <c r="I19" s="9"/>
+      <c r="I19" s="9">
+        <v>2</v>
+      </c>
       <c r="J19" s="9"/>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
@@ -1756,13 +1776,13 @@
     </row>
     <row r="20" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C20" s="7">
         <v>6</v>
       </c>
       <c r="D20" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E20" s="8"/>
       <c r="F20" s="7">
@@ -1774,9 +1794,11 @@
       <c r="H20" s="7">
         <v>5</v>
       </c>
-      <c r="I20" s="8"/>
-      <c r="J20" s="8"/>
-      <c r="K20" s="8"/>
+      <c r="I20" s="7">
+        <v>4</v>
+      </c>
+      <c r="J20" s="7"/>
+      <c r="K20" s="7"/>
       <c r="L20" s="8"/>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
@@ -1803,7 +1825,7 @@
         <v>1</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E21" s="9" t="s">
         <v>19</v>
@@ -1817,7 +1839,9 @@
       <c r="H21" s="9">
         <v>1</v>
       </c>
-      <c r="I21" s="9"/>
+      <c r="I21" s="9">
+        <v>0</v>
+      </c>
       <c r="J21" s="9"/>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
@@ -1840,13 +1864,13 @@
     </row>
     <row r="22" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C22" s="9">
         <v>3</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E22" s="9" t="s">
         <v>25</v>
@@ -1860,7 +1884,9 @@
       <c r="H22" s="9">
         <v>3</v>
       </c>
-      <c r="I22" s="9"/>
+      <c r="I22" s="9">
+        <v>3</v>
+      </c>
       <c r="J22" s="9"/>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
@@ -1903,7 +1929,9 @@
       <c r="H23" s="9">
         <v>1</v>
       </c>
-      <c r="I23" s="9"/>
+      <c r="I23" s="9">
+        <v>1</v>
+      </c>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
@@ -1927,13 +1955,13 @@
     <row r="24" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="10"/>
       <c r="B24" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C24" s="7">
         <v>5</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E24" s="8"/>
       <c r="F24" s="7">
@@ -1945,9 +1973,11 @@
       <c r="H24" s="7">
         <v>5</v>
       </c>
-      <c r="I24" s="8"/>
-      <c r="J24" s="8"/>
-      <c r="K24" s="8"/>
+      <c r="I24" s="7">
+        <v>4</v>
+      </c>
+      <c r="J24" s="7"/>
+      <c r="K24" s="7"/>
       <c r="L24" s="8"/>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
@@ -1975,7 +2005,7 @@
         <v>1</v>
       </c>
       <c r="D25" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E25" s="9" t="s">
         <v>19</v>
@@ -1989,7 +2019,9 @@
       <c r="H25" s="9">
         <v>1</v>
       </c>
-      <c r="I25" s="9"/>
+      <c r="I25" s="9">
+        <v>0</v>
+      </c>
       <c r="J25" s="9"/>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
@@ -2013,13 +2045,13 @@
     <row r="26" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="10"/>
       <c r="B26" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="9">
         <v>3</v>
       </c>
       <c r="D26" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E26" s="9" t="s">
         <v>25</v>
@@ -2033,7 +2065,9 @@
       <c r="H26" s="9">
         <v>3</v>
       </c>
-      <c r="I26" s="9"/>
+      <c r="I26" s="9">
+        <v>3</v>
+      </c>
       <c r="J26" s="9"/>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
@@ -2077,7 +2111,9 @@
       <c r="H27" s="9">
         <v>1</v>
       </c>
-      <c r="I27" s="9"/>
+      <c r="I27" s="9">
+        <v>1</v>
+      </c>
       <c r="J27" s="9"/>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
@@ -2130,13 +2166,13 @@
     </row>
     <row r="29" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C29" s="7">
         <v>6</v>
       </c>
       <c r="D29" s="12" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E29" s="8"/>
       <c r="F29" s="7">
@@ -2148,9 +2184,11 @@
       <c r="H29" s="7">
         <v>5</v>
       </c>
-      <c r="I29" s="8"/>
-      <c r="J29" s="8"/>
-      <c r="K29" s="8"/>
+      <c r="I29" s="7">
+        <v>4</v>
+      </c>
+      <c r="J29" s="7"/>
+      <c r="K29" s="7"/>
       <c r="L29" s="8"/>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
@@ -2177,7 +2215,7 @@
         <v>2</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>19</v>
@@ -2191,7 +2229,9 @@
       <c r="H30" s="9">
         <v>1</v>
       </c>
-      <c r="I30" s="9"/>
+      <c r="I30" s="9">
+        <v>0</v>
+      </c>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
@@ -2214,13 +2254,13 @@
     </row>
     <row r="31" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C31" s="9">
         <v>3</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>25</v>
@@ -2234,7 +2274,9 @@
       <c r="H31" s="9">
         <v>3</v>
       </c>
-      <c r="I31" s="9"/>
+      <c r="I31" s="9">
+        <v>3</v>
+      </c>
       <c r="J31" s="9"/>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
@@ -2277,7 +2319,9 @@
       <c r="H32" s="9">
         <v>1</v>
       </c>
-      <c r="I32" s="9"/>
+      <c r="I32" s="9">
+        <v>1</v>
+      </c>
       <c r="J32" s="9"/>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
@@ -2301,13 +2345,13 @@
     <row r="33" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="16"/>
       <c r="B33" s="7" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C33" s="7">
         <v>4</v>
       </c>
       <c r="D33" s="12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E33" s="8"/>
       <c r="F33" s="7">
@@ -2319,9 +2363,11 @@
       <c r="H33" s="7">
         <v>4</v>
       </c>
-      <c r="I33" s="8"/>
-      <c r="J33" s="8"/>
-      <c r="K33" s="8"/>
+      <c r="I33" s="7">
+        <v>4</v>
+      </c>
+      <c r="J33" s="7"/>
+      <c r="K33" s="7"/>
       <c r="L33" s="8"/>
       <c r="M33" s="11"/>
       <c r="N33" s="11"/>
@@ -2342,13 +2388,13 @@
     </row>
     <row r="34" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C34" s="9">
         <v>3</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>25</v>
@@ -2362,7 +2408,9 @@
       <c r="H34" s="9">
         <v>3</v>
       </c>
-      <c r="I34" s="9"/>
+      <c r="I34" s="9">
+        <v>3</v>
+      </c>
       <c r="J34" s="9"/>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
@@ -2405,7 +2453,9 @@
       <c r="H35" s="9">
         <v>1</v>
       </c>
-      <c r="I35" s="9"/>
+      <c r="I35" s="9">
+        <v>1</v>
+      </c>
       <c r="J35" s="9"/>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
@@ -2446,9 +2496,11 @@
       <c r="H36" s="7">
         <v>4</v>
       </c>
-      <c r="I36" s="8"/>
-      <c r="J36" s="8"/>
-      <c r="K36" s="8"/>
+      <c r="I36" s="7">
+        <v>4</v>
+      </c>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
       <c r="L36" s="8"/>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
@@ -2469,13 +2521,13 @@
     </row>
     <row r="37" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C37" s="9">
         <v>3</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E37" s="9" t="s">
         <v>25</v>
@@ -2489,7 +2541,9 @@
       <c r="H37" s="9">
         <v>3</v>
       </c>
-      <c r="I37" s="9"/>
+      <c r="I37" s="9">
+        <v>3</v>
+      </c>
       <c r="J37" s="9"/>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
@@ -2532,7 +2586,9 @@
       <c r="H38" s="9">
         <v>1</v>
       </c>
-      <c r="I38" s="9"/>
+      <c r="I38" s="9">
+        <v>1</v>
+      </c>
       <c r="J38" s="9"/>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
@@ -2573,9 +2629,11 @@
       <c r="H39" s="7">
         <v>4</v>
       </c>
-      <c r="I39" s="8"/>
-      <c r="J39" s="8"/>
-      <c r="K39" s="8"/>
+      <c r="I39" s="7">
+        <v>4</v>
+      </c>
+      <c r="J39" s="7"/>
+      <c r="K39" s="7"/>
       <c r="L39" s="8"/>
       <c r="M39" s="11"/>
       <c r="N39" s="11"/>
@@ -2596,13 +2654,13 @@
     </row>
     <row r="40" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C40" s="9">
         <v>3</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E40" s="9" t="s">
         <v>25</v>
@@ -2616,7 +2674,9 @@
       <c r="H40" s="9">
         <v>3</v>
       </c>
-      <c r="I40" s="9"/>
+      <c r="I40" s="9">
+        <v>3</v>
+      </c>
       <c r="J40" s="9"/>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
@@ -2659,7 +2719,9 @@
       <c r="H41" s="9">
         <v>1</v>
       </c>
-      <c r="I41" s="9"/>
+      <c r="I41" s="9">
+        <v>1</v>
+      </c>
       <c r="J41" s="9"/>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
@@ -2688,7 +2750,7 @@
         <v>4</v>
       </c>
       <c r="D42" s="12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E42" s="12"/>
       <c r="F42" s="7">
@@ -2700,9 +2762,11 @@
       <c r="H42" s="17">
         <v>4</v>
       </c>
-      <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
-      <c r="K42" s="12"/>
+      <c r="I42" s="17">
+        <v>4</v>
+      </c>
+      <c r="J42" s="14"/>
+      <c r="K42" s="14"/>
       <c r="L42" s="12"/>
       <c r="M42" s="11"/>
       <c r="N42" s="11"/>
@@ -2723,13 +2787,13 @@
     </row>
     <row r="43" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C43" s="9">
         <v>3</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E43" s="9" t="s">
         <v>25</v>
@@ -2743,7 +2807,9 @@
       <c r="H43" s="9">
         <v>3</v>
       </c>
-      <c r="I43" s="9"/>
+      <c r="I43" s="9">
+        <v>3</v>
+      </c>
       <c r="J43" s="9"/>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
@@ -2786,7 +2852,9 @@
       <c r="H44" s="9">
         <v>1</v>
       </c>
-      <c r="I44" s="9"/>
+      <c r="I44" s="9">
+        <v>1</v>
+      </c>
       <c r="J44" s="9"/>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
@@ -2815,7 +2883,7 @@
         <v>4</v>
       </c>
       <c r="D45" s="12" t="s">
-        <v>21</v>
+        <v>39</v>
       </c>
       <c r="E45" s="12"/>
       <c r="F45" s="7">
@@ -2827,9 +2895,11 @@
       <c r="H45" s="17">
         <v>4</v>
       </c>
-      <c r="I45" s="12"/>
-      <c r="J45" s="12"/>
-      <c r="K45" s="12"/>
+      <c r="I45" s="17">
+        <v>2.5</v>
+      </c>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
       <c r="L45" s="12"/>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
@@ -2850,13 +2920,13 @@
     </row>
     <row r="46" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C46" s="9">
         <v>3</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="E46" s="9" t="s">
         <v>25</v>
@@ -2870,7 +2940,9 @@
       <c r="H46" s="9">
         <v>3</v>
       </c>
-      <c r="I46" s="9"/>
+      <c r="I46" s="9">
+        <v>2</v>
+      </c>
       <c r="J46" s="9"/>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
@@ -2913,7 +2985,9 @@
       <c r="H47" s="9">
         <v>1</v>
       </c>
-      <c r="I47" s="9"/>
+      <c r="I47" s="9">
+        <v>0.5</v>
+      </c>
       <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
@@ -2954,7 +3028,7 @@
         <v>53</v>
       </c>
       <c r="I48" s="5">
-        <v>0</v>
+        <v>43.5</v>
       </c>
       <c r="J48" s="5">
         <v>0</v>
@@ -3013,27 +3087,27 @@
       <c r="AB49" s="4"/>
     </row>
     <row r="50" spans="2:28" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="20"/>
-      <c r="C50" s="20"/>
-      <c r="D50" s="20"/>
-      <c r="E50" s="20"/>
-      <c r="F50" s="20"/>
-      <c r="G50" s="20"/>
-      <c r="H50" s="20"/>
-      <c r="I50" s="20"/>
-      <c r="J50" s="20"/>
-      <c r="K50" s="20"/>
-      <c r="L50" s="20"/>
-      <c r="M50" s="20"/>
-      <c r="N50" s="20"/>
-      <c r="O50" s="20"/>
-      <c r="P50" s="20"/>
-      <c r="Q50" s="20"/>
-      <c r="R50" s="20"/>
-      <c r="S50" s="20"/>
-      <c r="T50" s="20"/>
-      <c r="U50" s="20"/>
-      <c r="V50" s="20"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="19"/>
+      <c r="D50" s="19"/>
+      <c r="E50" s="19"/>
+      <c r="F50" s="19"/>
+      <c r="G50" s="19"/>
+      <c r="H50" s="19"/>
+      <c r="I50" s="19"/>
+      <c r="J50" s="19"/>
+      <c r="K50" s="19"/>
+      <c r="L50" s="19"/>
+      <c r="M50" s="19"/>
+      <c r="N50" s="19"/>
+      <c r="O50" s="19"/>
+      <c r="P50" s="19"/>
+      <c r="Q50" s="19"/>
+      <c r="R50" s="19"/>
+      <c r="S50" s="19"/>
+      <c r="T50" s="19"/>
+      <c r="U50" s="19"/>
+      <c r="V50" s="19"/>
       <c r="W50" s="4"/>
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>

</xml_diff>

<commit_message>
Updating Sprint 2 Backlog (day 4)
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\OneDrive\Documents\University\Third Year\Agile\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{586F1A4F-9DD0-416D-B961-7BC431B036C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D69ED37E-E183-43A0-B7D9-127C9407EB8D}"/>
+  <xr:revisionPtr revIDLastSave="135" documentId="8_{586F1A4F-9DD0-416D-B961-7BC431B036C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0469C1B-59BA-4944-99BD-6B5E9A1577AA}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -463,10 +463,10 @@
                   <c:v>53</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>43.5</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>0</c:v>
@@ -953,8 +953,8 @@
   <dimension ref="A1:AC144"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I18" sqref="I18"/>
+      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B50" sqref="B50:V50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1082,7 +1082,9 @@
       <c r="I3" s="7">
         <v>0</v>
       </c>
-      <c r="J3" s="7"/>
+      <c r="J3" s="7">
+        <v>0</v>
+      </c>
       <c r="K3" s="7"/>
       <c r="L3" s="8"/>
       <c r="M3" s="4"/>
@@ -1157,7 +1159,9 @@
       <c r="I5" s="7">
         <v>0</v>
       </c>
-      <c r="J5" s="7"/>
+      <c r="J5" s="7">
+        <v>0</v>
+      </c>
       <c r="K5" s="7"/>
       <c r="L5" s="8"/>
       <c r="M5" s="11"/>
@@ -1232,7 +1236,9 @@
       <c r="I7" s="7">
         <v>0</v>
       </c>
-      <c r="J7" s="7"/>
+      <c r="J7" s="7">
+        <v>0</v>
+      </c>
       <c r="K7" s="7"/>
       <c r="L7" s="8"/>
       <c r="M7" s="4"/>
@@ -1306,7 +1312,9 @@
       <c r="I9" s="7">
         <v>4</v>
       </c>
-      <c r="J9" s="7"/>
+      <c r="J9" s="7">
+        <v>2</v>
+      </c>
       <c r="K9" s="7"/>
       <c r="L9" s="8"/>
       <c r="M9" s="4"/>
@@ -1351,7 +1359,9 @@
       <c r="I10" s="9">
         <v>0</v>
       </c>
-      <c r="J10" s="9"/>
+      <c r="J10" s="9">
+        <v>0</v>
+      </c>
       <c r="K10" s="9"/>
       <c r="L10" s="9"/>
       <c r="M10" s="4"/>
@@ -1396,7 +1406,9 @@
       <c r="I11" s="9">
         <v>3</v>
       </c>
-      <c r="J11" s="9"/>
+      <c r="J11" s="9">
+        <v>2</v>
+      </c>
       <c r="K11" s="9"/>
       <c r="L11" s="9"/>
       <c r="M11" s="4"/>
@@ -1441,7 +1453,9 @@
       <c r="I12" s="9">
         <v>1</v>
       </c>
-      <c r="J12" s="9"/>
+      <c r="J12" s="9">
+        <v>0</v>
+      </c>
       <c r="K12" s="9"/>
       <c r="L12" s="9"/>
       <c r="M12" s="4"/>
@@ -1484,7 +1498,9 @@
       <c r="I13" s="7">
         <v>4</v>
       </c>
-      <c r="J13" s="7"/>
+      <c r="J13" s="7">
+        <v>4</v>
+      </c>
       <c r="K13" s="7"/>
       <c r="L13" s="8"/>
       <c r="M13" s="4"/>
@@ -1529,7 +1545,9 @@
       <c r="I14" s="9">
         <v>0</v>
       </c>
-      <c r="J14" s="9"/>
+      <c r="J14" s="9">
+        <v>0</v>
+      </c>
       <c r="K14" s="9"/>
       <c r="L14" s="9"/>
       <c r="M14" s="9"/>
@@ -1575,7 +1593,9 @@
       <c r="I15" s="9">
         <v>3</v>
       </c>
-      <c r="J15" s="9"/>
+      <c r="J15" s="9">
+        <v>3</v>
+      </c>
       <c r="K15" s="9"/>
       <c r="L15" s="9"/>
       <c r="M15" s="13"/>
@@ -1621,7 +1641,9 @@
       <c r="I16" s="9">
         <v>1</v>
       </c>
-      <c r="J16" s="9"/>
+      <c r="J16" s="9">
+        <v>1</v>
+      </c>
       <c r="K16" s="9"/>
       <c r="L16" s="9"/>
       <c r="M16" s="4"/>
@@ -1664,7 +1686,9 @@
       <c r="I17" s="7">
         <v>5</v>
       </c>
-      <c r="J17" s="7"/>
+      <c r="J17" s="7">
+        <v>3</v>
+      </c>
       <c r="K17" s="7"/>
       <c r="L17" s="8"/>
       <c r="M17" s="4"/>
@@ -1709,7 +1733,9 @@
       <c r="I18" s="9">
         <v>3</v>
       </c>
-      <c r="J18" s="9"/>
+      <c r="J18" s="9">
+        <v>2</v>
+      </c>
       <c r="K18" s="9"/>
       <c r="L18" s="9"/>
       <c r="M18" s="4"/>
@@ -1754,7 +1780,9 @@
       <c r="I19" s="9">
         <v>2</v>
       </c>
-      <c r="J19" s="9"/>
+      <c r="J19" s="9">
+        <v>1</v>
+      </c>
       <c r="K19" s="9"/>
       <c r="L19" s="9"/>
       <c r="M19" s="4"/>
@@ -1797,7 +1825,9 @@
       <c r="I20" s="7">
         <v>4</v>
       </c>
-      <c r="J20" s="7"/>
+      <c r="J20" s="7">
+        <v>4</v>
+      </c>
       <c r="K20" s="7"/>
       <c r="L20" s="8"/>
       <c r="M20" s="4"/>
@@ -1842,7 +1872,9 @@
       <c r="I21" s="9">
         <v>0</v>
       </c>
-      <c r="J21" s="9"/>
+      <c r="J21" s="9">
+        <v>0</v>
+      </c>
       <c r="K21" s="9"/>
       <c r="L21" s="9"/>
       <c r="M21" s="4"/>
@@ -1887,7 +1919,9 @@
       <c r="I22" s="9">
         <v>3</v>
       </c>
-      <c r="J22" s="9"/>
+      <c r="J22" s="9">
+        <v>3</v>
+      </c>
       <c r="K22" s="9"/>
       <c r="L22" s="9"/>
       <c r="M22" s="4"/>
@@ -1932,7 +1966,9 @@
       <c r="I23" s="9">
         <v>1</v>
       </c>
-      <c r="J23" s="9"/>
+      <c r="J23" s="9">
+        <v>1</v>
+      </c>
       <c r="K23" s="9"/>
       <c r="L23" s="9"/>
       <c r="M23" s="4"/>
@@ -1976,7 +2012,9 @@
       <c r="I24" s="7">
         <v>4</v>
       </c>
-      <c r="J24" s="7"/>
+      <c r="J24" s="7">
+        <v>3</v>
+      </c>
       <c r="K24" s="7"/>
       <c r="L24" s="8"/>
       <c r="M24" s="11"/>
@@ -2022,7 +2060,9 @@
       <c r="I25" s="9">
         <v>0</v>
       </c>
-      <c r="J25" s="9"/>
+      <c r="J25" s="9">
+        <v>0</v>
+      </c>
       <c r="K25" s="9"/>
       <c r="L25" s="9"/>
       <c r="M25" s="11"/>
@@ -2068,7 +2108,9 @@
       <c r="I26" s="9">
         <v>3</v>
       </c>
-      <c r="J26" s="9"/>
+      <c r="J26" s="9">
+        <v>2</v>
+      </c>
       <c r="K26" s="9"/>
       <c r="L26" s="9"/>
       <c r="M26" s="11"/>
@@ -2114,7 +2156,9 @@
       <c r="I27" s="9">
         <v>1</v>
       </c>
-      <c r="J27" s="9"/>
+      <c r="J27" s="9">
+        <v>1</v>
+      </c>
       <c r="K27" s="9"/>
       <c r="L27" s="9"/>
       <c r="M27" s="11"/>
@@ -2187,7 +2231,9 @@
       <c r="I29" s="7">
         <v>4</v>
       </c>
-      <c r="J29" s="7"/>
+      <c r="J29" s="7">
+        <v>4</v>
+      </c>
       <c r="K29" s="7"/>
       <c r="L29" s="8"/>
       <c r="M29" s="4"/>
@@ -2232,7 +2278,9 @@
       <c r="I30" s="9">
         <v>0</v>
       </c>
-      <c r="J30" s="9"/>
+      <c r="J30" s="9">
+        <v>0</v>
+      </c>
       <c r="K30" s="9"/>
       <c r="L30" s="9"/>
       <c r="M30" s="4"/>
@@ -2277,7 +2325,9 @@
       <c r="I31" s="9">
         <v>3</v>
       </c>
-      <c r="J31" s="9"/>
+      <c r="J31" s="9">
+        <v>3</v>
+      </c>
       <c r="K31" s="9"/>
       <c r="L31" s="9"/>
       <c r="M31" s="4"/>
@@ -2322,7 +2372,9 @@
       <c r="I32" s="9">
         <v>1</v>
       </c>
-      <c r="J32" s="9"/>
+      <c r="J32" s="9">
+        <v>1</v>
+      </c>
       <c r="K32" s="9"/>
       <c r="L32" s="9"/>
       <c r="M32" s="4"/>
@@ -2366,7 +2418,9 @@
       <c r="I33" s="7">
         <v>4</v>
       </c>
-      <c r="J33" s="7"/>
+      <c r="J33" s="7">
+        <v>4</v>
+      </c>
       <c r="K33" s="7"/>
       <c r="L33" s="8"/>
       <c r="M33" s="11"/>
@@ -2411,7 +2465,9 @@
       <c r="I34" s="9">
         <v>3</v>
       </c>
-      <c r="J34" s="9"/>
+      <c r="J34" s="9">
+        <v>3</v>
+      </c>
       <c r="K34" s="9"/>
       <c r="L34" s="9"/>
       <c r="M34" s="11"/>
@@ -2456,7 +2512,9 @@
       <c r="I35" s="9">
         <v>1</v>
       </c>
-      <c r="J35" s="9"/>
+      <c r="J35" s="9">
+        <v>1</v>
+      </c>
       <c r="K35" s="9"/>
       <c r="L35" s="9"/>
       <c r="M35" s="11"/>
@@ -2499,7 +2557,9 @@
       <c r="I36" s="7">
         <v>4</v>
       </c>
-      <c r="J36" s="7"/>
+      <c r="J36" s="7">
+        <v>4</v>
+      </c>
       <c r="K36" s="7"/>
       <c r="L36" s="8"/>
       <c r="M36" s="11"/>
@@ -2544,7 +2604,9 @@
       <c r="I37" s="9">
         <v>3</v>
       </c>
-      <c r="J37" s="9"/>
+      <c r="J37" s="9">
+        <v>3</v>
+      </c>
       <c r="K37" s="9"/>
       <c r="L37" s="9"/>
       <c r="M37" s="11"/>
@@ -2589,7 +2651,9 @@
       <c r="I38" s="9">
         <v>1</v>
       </c>
-      <c r="J38" s="9"/>
+      <c r="J38" s="9">
+        <v>1</v>
+      </c>
       <c r="K38" s="9"/>
       <c r="L38" s="9"/>
       <c r="M38" s="11"/>
@@ -2632,7 +2696,9 @@
       <c r="I39" s="7">
         <v>4</v>
       </c>
-      <c r="J39" s="7"/>
+      <c r="J39" s="7">
+        <v>3</v>
+      </c>
       <c r="K39" s="7"/>
       <c r="L39" s="8"/>
       <c r="M39" s="11"/>
@@ -2677,7 +2743,9 @@
       <c r="I40" s="9">
         <v>3</v>
       </c>
-      <c r="J40" s="9"/>
+      <c r="J40" s="9">
+        <v>2</v>
+      </c>
       <c r="K40" s="9"/>
       <c r="L40" s="9"/>
       <c r="M40" s="11"/>
@@ -2722,7 +2790,9 @@
       <c r="I41" s="9">
         <v>1</v>
       </c>
-      <c r="J41" s="9"/>
+      <c r="J41" s="9">
+        <v>1</v>
+      </c>
       <c r="K41" s="9"/>
       <c r="L41" s="9"/>
       <c r="M41" s="11"/>
@@ -2765,7 +2835,9 @@
       <c r="I42" s="17">
         <v>4</v>
       </c>
-      <c r="J42" s="14"/>
+      <c r="J42" s="17">
+        <v>2</v>
+      </c>
       <c r="K42" s="14"/>
       <c r="L42" s="12"/>
       <c r="M42" s="11"/>
@@ -2810,7 +2882,9 @@
       <c r="I43" s="9">
         <v>3</v>
       </c>
-      <c r="J43" s="9"/>
+      <c r="J43" s="9">
+        <v>2</v>
+      </c>
       <c r="K43" s="9"/>
       <c r="L43" s="9"/>
       <c r="M43" s="11"/>
@@ -2855,7 +2929,9 @@
       <c r="I44" s="9">
         <v>1</v>
       </c>
-      <c r="J44" s="9"/>
+      <c r="J44" s="9">
+        <v>0</v>
+      </c>
       <c r="K44" s="9"/>
       <c r="L44" s="9"/>
       <c r="M44" s="11"/>
@@ -2896,9 +2972,11 @@
         <v>4</v>
       </c>
       <c r="I45" s="17">
-        <v>2.5</v>
-      </c>
-      <c r="J45" s="14"/>
+        <v>3</v>
+      </c>
+      <c r="J45" s="17">
+        <v>1.5</v>
+      </c>
       <c r="K45" s="14"/>
       <c r="L45" s="12"/>
       <c r="M45" s="11"/>
@@ -2943,7 +3021,9 @@
       <c r="I46" s="9">
         <v>2</v>
       </c>
-      <c r="J46" s="9"/>
+      <c r="J46" s="9">
+        <v>1</v>
+      </c>
       <c r="K46" s="9"/>
       <c r="L46" s="9"/>
       <c r="M46" s="11"/>
@@ -2986,9 +3066,11 @@
         <v>1</v>
       </c>
       <c r="I47" s="9">
+        <v>1</v>
+      </c>
+      <c r="J47" s="9">
         <v>0.5</v>
       </c>
-      <c r="J47" s="9"/>
       <c r="K47" s="9"/>
       <c r="L47" s="9"/>
       <c r="M47" s="11"/>
@@ -3028,10 +3110,10 @@
         <v>53</v>
       </c>
       <c r="I48" s="5">
-        <v>43.5</v>
+        <v>44</v>
       </c>
       <c r="J48" s="5">
-        <v>0</v>
+        <v>34.5</v>
       </c>
       <c r="K48" s="5">
         <v>0</v>

</xml_diff>

<commit_message>
Updating Sprint 2 Backlog (Day 5)
</commit_message>
<xml_diff>
--- a/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
+++ b/Sprint 2/Sprint_Backlog/Sprint 2 Backlog.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sarah\OneDrive\Documents\University\Third Year\Agile\Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="135" documentId="8_{586F1A4F-9DD0-416D-B961-7BC431B036C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D0469C1B-59BA-4944-99BD-6B5E9A1577AA}"/>
+  <xr:revisionPtr revIDLastSave="282" documentId="8_{586F1A4F-9DD0-416D-B961-7BC431B036C4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{D1E03663-F9E0-4250-8426-6AA63AFC1D05}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Agile Sprint Backlog" sheetId="5" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$V$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">'Agile Sprint Backlog'!$B$2:$V$47</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -294,7 +294,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -334,6 +334,9 @@
     <xf numFmtId="0" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -449,7 +452,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'Agile Sprint Backlog'!$F$48:$L$48</c:f>
+              <c:f>'Agile Sprint Backlog'!$F$47:$L$47</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="7"/>
@@ -469,10 +472,10 @@
                   <c:v>34.5</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0</c:v>
+                  <c:v>17</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -950,11 +953,11 @@
     <tabColor theme="3"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:AC144"/>
+  <dimension ref="A1:AC143"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A41" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B50" sqref="B50:V50"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="68" zoomScaleNormal="70" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -976,29 +979,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" ht="50.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="18" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="18"/>
-      <c r="I1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
+      <c r="B1" s="19" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="19"/>
+      <c r="D1" s="19"/>
+      <c r="E1" s="19"/>
+      <c r="F1" s="19"/>
+      <c r="G1" s="19"/>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="19"/>
+      <c r="K1" s="19"/>
+      <c r="L1" s="19"/>
+      <c r="M1" s="19"/>
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="19"/>
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="19"/>
       <c r="W1" s="4"/>
       <c r="X1" s="4"/>
       <c r="Y1" s="4"/>
@@ -1085,8 +1088,12 @@
       <c r="J3" s="7">
         <v>0</v>
       </c>
-      <c r="K3" s="7"/>
-      <c r="L3" s="8"/>
+      <c r="K3" s="7">
+        <v>0</v>
+      </c>
+      <c r="L3" s="7">
+        <v>0</v>
+      </c>
       <c r="M3" s="4"/>
       <c r="N3" s="4"/>
       <c r="O3" s="4"/>
@@ -1115,7 +1122,7 @@
       <c r="I4" s="9"/>
       <c r="J4" s="9"/>
       <c r="K4" s="9"/>
-      <c r="L4" s="9"/>
+      <c r="L4" s="18"/>
       <c r="M4" s="4"/>
       <c r="N4" s="4"/>
       <c r="O4" s="4"/>
@@ -1162,8 +1169,12 @@
       <c r="J5" s="7">
         <v>0</v>
       </c>
-      <c r="K5" s="7"/>
-      <c r="L5" s="8"/>
+      <c r="K5" s="7">
+        <v>0</v>
+      </c>
+      <c r="L5" s="7">
+        <v>0</v>
+      </c>
       <c r="M5" s="11"/>
       <c r="N5" s="11"/>
       <c r="O5" s="11"/>
@@ -1193,7 +1204,7 @@
       <c r="I6" s="9"/>
       <c r="J6" s="9"/>
       <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
+      <c r="L6" s="18"/>
       <c r="M6" s="4"/>
       <c r="N6" s="4"/>
       <c r="O6" s="4"/>
@@ -1222,7 +1233,7 @@
         <v>18</v>
       </c>
       <c r="E7" s="8" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F7" s="7">
         <v>5</v>
@@ -1239,8 +1250,12 @@
       <c r="J7" s="7">
         <v>0</v>
       </c>
-      <c r="K7" s="7"/>
-      <c r="L7" s="8"/>
+      <c r="K7" s="7">
+        <v>0</v>
+      </c>
+      <c r="L7" s="7">
+        <v>0</v>
+      </c>
       <c r="M7" s="4"/>
       <c r="N7" s="4"/>
       <c r="O7" s="4"/>
@@ -1269,7 +1284,7 @@
       <c r="I8" s="9"/>
       <c r="J8" s="9"/>
       <c r="K8" s="9"/>
-      <c r="L8" s="9"/>
+      <c r="L8" s="18"/>
       <c r="M8" s="4"/>
       <c r="N8" s="4"/>
       <c r="O8" s="4"/>
@@ -1315,8 +1330,12 @@
       <c r="J9" s="7">
         <v>2</v>
       </c>
-      <c r="K9" s="7"/>
-      <c r="L9" s="8"/>
+      <c r="K9" s="7">
+        <v>2</v>
+      </c>
+      <c r="L9" s="7">
+        <v>2</v>
+      </c>
       <c r="M9" s="4"/>
       <c r="N9" s="4"/>
       <c r="O9" s="4"/>
@@ -1345,7 +1364,7 @@
         <v>22</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F10" s="9">
         <v>1</v>
@@ -1362,8 +1381,12 @@
       <c r="J10" s="9">
         <v>0</v>
       </c>
-      <c r="K10" s="9"/>
-      <c r="L10" s="9"/>
+      <c r="K10" s="9">
+        <v>0</v>
+      </c>
+      <c r="L10" s="9">
+        <v>0</v>
+      </c>
       <c r="M10" s="4"/>
       <c r="N10" s="4"/>
       <c r="O10" s="4"/>
@@ -1392,7 +1415,7 @@
         <v>24</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F11" s="9">
         <v>3</v>
@@ -1409,8 +1432,12 @@
       <c r="J11" s="9">
         <v>2</v>
       </c>
-      <c r="K11" s="9"/>
-      <c r="L11" s="9"/>
+      <c r="K11" s="9">
+        <v>2</v>
+      </c>
+      <c r="L11" s="9">
+        <v>2</v>
+      </c>
       <c r="M11" s="4"/>
       <c r="N11" s="4"/>
       <c r="O11" s="4"/>
@@ -1439,7 +1466,7 @@
         <v>27</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F12" s="9">
         <v>1</v>
@@ -1456,8 +1483,12 @@
       <c r="J12" s="9">
         <v>0</v>
       </c>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
+      <c r="K12" s="9">
+        <v>0</v>
+      </c>
+      <c r="L12" s="9">
+        <v>0</v>
+      </c>
       <c r="M12" s="4"/>
       <c r="N12" s="4"/>
       <c r="O12" s="4"/>
@@ -1501,8 +1532,12 @@
       <c r="J13" s="7">
         <v>4</v>
       </c>
-      <c r="K13" s="7"/>
-      <c r="L13" s="8"/>
+      <c r="K13" s="7">
+        <v>2</v>
+      </c>
+      <c r="L13" s="7">
+        <v>2</v>
+      </c>
       <c r="M13" s="4"/>
       <c r="N13" s="4"/>
       <c r="O13" s="4"/>
@@ -1531,7 +1566,7 @@
         <v>22</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F14" s="9">
         <v>2</v>
@@ -1548,8 +1583,12 @@
       <c r="J14" s="9">
         <v>0</v>
       </c>
-      <c r="K14" s="9"/>
-      <c r="L14" s="9"/>
+      <c r="K14" s="9">
+        <v>0</v>
+      </c>
+      <c r="L14" s="9">
+        <v>0</v>
+      </c>
       <c r="M14" s="9"/>
       <c r="N14" s="11"/>
       <c r="O14" s="11"/>
@@ -1579,7 +1618,7 @@
         <v>24</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="F15" s="9">
         <v>3</v>
@@ -1596,8 +1635,12 @@
       <c r="J15" s="9">
         <v>3</v>
       </c>
-      <c r="K15" s="9"/>
-      <c r="L15" s="9"/>
+      <c r="K15" s="9">
+        <v>2</v>
+      </c>
+      <c r="L15" s="9">
+        <v>2</v>
+      </c>
       <c r="M15" s="13"/>
       <c r="N15" s="4"/>
       <c r="O15" s="4"/>
@@ -1627,7 +1670,7 @@
         <v>27</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F16" s="9">
         <v>1</v>
@@ -1644,8 +1687,12 @@
       <c r="J16" s="9">
         <v>1</v>
       </c>
-      <c r="K16" s="9"/>
-      <c r="L16" s="9"/>
+      <c r="K16" s="9">
+        <v>0</v>
+      </c>
+      <c r="L16" s="9">
+        <v>0</v>
+      </c>
       <c r="M16" s="4"/>
       <c r="N16" s="4"/>
       <c r="O16" s="4"/>
@@ -1689,8 +1736,12 @@
       <c r="J17" s="7">
         <v>3</v>
       </c>
-      <c r="K17" s="7"/>
-      <c r="L17" s="8"/>
+      <c r="K17" s="7">
+        <v>0</v>
+      </c>
+      <c r="L17" s="7">
+        <v>0</v>
+      </c>
       <c r="M17" s="4"/>
       <c r="N17" s="4"/>
       <c r="O17" s="4"/>
@@ -1719,7 +1770,7 @@
         <v>24</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F18" s="9">
         <v>3</v>
@@ -1736,8 +1787,12 @@
       <c r="J18" s="9">
         <v>2</v>
       </c>
-      <c r="K18" s="9"/>
-      <c r="L18" s="9"/>
+      <c r="K18" s="9">
+        <v>0</v>
+      </c>
+      <c r="L18" s="9">
+        <v>0</v>
+      </c>
       <c r="M18" s="4"/>
       <c r="N18" s="4"/>
       <c r="O18" s="4"/>
@@ -1766,7 +1821,7 @@
         <v>16</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F19" s="9">
         <v>2</v>
@@ -1783,8 +1838,12 @@
       <c r="J19" s="9">
         <v>1</v>
       </c>
-      <c r="K19" s="9"/>
-      <c r="L19" s="9"/>
+      <c r="K19" s="9">
+        <v>0</v>
+      </c>
+      <c r="L19" s="9">
+        <v>0</v>
+      </c>
       <c r="M19" s="4"/>
       <c r="N19" s="4"/>
       <c r="O19" s="4"/>
@@ -1828,8 +1887,12 @@
       <c r="J20" s="7">
         <v>4</v>
       </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
+      <c r="K20" s="7">
+        <v>4</v>
+      </c>
+      <c r="L20" s="7">
+        <v>4</v>
+      </c>
       <c r="M20" s="4"/>
       <c r="N20" s="4"/>
       <c r="O20" s="4"/>
@@ -1858,7 +1921,7 @@
         <v>22</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F21" s="9">
         <v>1</v>
@@ -1875,8 +1938,12 @@
       <c r="J21" s="9">
         <v>0</v>
       </c>
-      <c r="K21" s="9"/>
-      <c r="L21" s="9"/>
+      <c r="K21" s="9">
+        <v>0</v>
+      </c>
+      <c r="L21" s="9">
+        <v>0</v>
+      </c>
       <c r="M21" s="4"/>
       <c r="N21" s="4"/>
       <c r="O21" s="4"/>
@@ -1922,8 +1989,12 @@
       <c r="J22" s="9">
         <v>3</v>
       </c>
-      <c r="K22" s="9"/>
-      <c r="L22" s="9"/>
+      <c r="K22" s="9">
+        <v>3</v>
+      </c>
+      <c r="L22" s="9">
+        <v>3</v>
+      </c>
       <c r="M22" s="4"/>
       <c r="N22" s="4"/>
       <c r="O22" s="4"/>
@@ -1969,8 +2040,12 @@
       <c r="J23" s="9">
         <v>1</v>
       </c>
-      <c r="K23" s="9"/>
-      <c r="L23" s="9"/>
+      <c r="K23" s="9">
+        <v>1</v>
+      </c>
+      <c r="L23" s="9">
+        <v>1</v>
+      </c>
       <c r="M23" s="4"/>
       <c r="N23" s="4"/>
       <c r="O23" s="4"/>
@@ -2015,8 +2090,12 @@
       <c r="J24" s="7">
         <v>3</v>
       </c>
-      <c r="K24" s="7"/>
-      <c r="L24" s="8"/>
+      <c r="K24" s="7">
+        <v>0</v>
+      </c>
+      <c r="L24" s="7">
+        <v>0</v>
+      </c>
       <c r="M24" s="11"/>
       <c r="N24" s="11"/>
       <c r="O24" s="11"/>
@@ -2046,7 +2125,7 @@
         <v>22</v>
       </c>
       <c r="E25" s="9" t="s">
-        <v>19</v>
+        <v>14</v>
       </c>
       <c r="F25" s="9">
         <v>1</v>
@@ -2063,8 +2142,12 @@
       <c r="J25" s="9">
         <v>0</v>
       </c>
-      <c r="K25" s="9"/>
-      <c r="L25" s="9"/>
+      <c r="K25" s="9">
+        <v>0</v>
+      </c>
+      <c r="L25" s="9">
+        <v>0</v>
+      </c>
       <c r="M25" s="11"/>
       <c r="N25" s="11"/>
       <c r="O25" s="11"/>
@@ -2094,7 +2177,7 @@
         <v>24</v>
       </c>
       <c r="E26" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F26" s="9">
         <v>3</v>
@@ -2111,8 +2194,12 @@
       <c r="J26" s="9">
         <v>2</v>
       </c>
-      <c r="K26" s="9"/>
-      <c r="L26" s="9"/>
+      <c r="K26" s="9">
+        <v>0</v>
+      </c>
+      <c r="L26" s="9">
+        <v>0</v>
+      </c>
       <c r="M26" s="11"/>
       <c r="N26" s="11"/>
       <c r="O26" s="11"/>
@@ -2142,7 +2229,7 @@
         <v>27</v>
       </c>
       <c r="E27" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F27" s="9">
         <v>1</v>
@@ -2159,8 +2246,12 @@
       <c r="J27" s="9">
         <v>1</v>
       </c>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
+      <c r="K27" s="9">
+        <v>0</v>
+      </c>
+      <c r="L27" s="9">
+        <v>0</v>
+      </c>
       <c r="M27" s="11"/>
       <c r="N27" s="11"/>
       <c r="O27" s="11"/>
@@ -2179,63 +2270,88 @@
       <c r="AB27" s="11"/>
     </row>
     <row r="28" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="10"/>
-      <c r="B28" s="9"/>
-      <c r="C28" s="9"/>
-      <c r="D28" s="9"/>
-      <c r="E28" s="9"/>
-      <c r="F28" s="9"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="9"/>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="9"/>
-      <c r="L28" s="9"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
-      <c r="AB28" s="11"/>
+      <c r="B28" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C28" s="7">
+        <v>6</v>
+      </c>
+      <c r="D28" s="12" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" s="8"/>
+      <c r="F28" s="7">
+        <v>6</v>
+      </c>
+      <c r="G28" s="7">
+        <v>6</v>
+      </c>
+      <c r="H28" s="7">
+        <v>5</v>
+      </c>
+      <c r="I28" s="7">
+        <v>4</v>
+      </c>
+      <c r="J28" s="7">
+        <v>4</v>
+      </c>
+      <c r="K28" s="7">
+        <v>3</v>
+      </c>
+      <c r="L28" s="7">
+        <v>3</v>
+      </c>
+      <c r="M28" s="4"/>
+      <c r="N28" s="4"/>
+      <c r="O28" s="4"/>
+      <c r="P28" s="4"/>
+      <c r="Q28" s="4"/>
+      <c r="R28" s="4"/>
+      <c r="S28" s="4"/>
+      <c r="T28" s="4"/>
+      <c r="U28" s="4"/>
+      <c r="V28" s="4"/>
+      <c r="W28" s="4"/>
+      <c r="X28" s="4"/>
+      <c r="Y28" s="4"/>
+      <c r="Z28" s="4"/>
+      <c r="AA28" s="4"/>
+      <c r="AB28" s="4"/>
     </row>
     <row r="29" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B29" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="7">
-        <v>6</v>
-      </c>
-      <c r="D29" s="12" t="s">
-        <v>37</v>
-      </c>
-      <c r="E29" s="8"/>
-      <c r="F29" s="7">
-        <v>6</v>
-      </c>
-      <c r="G29" s="7">
-        <v>6</v>
-      </c>
-      <c r="H29" s="7">
-        <v>5</v>
-      </c>
-      <c r="I29" s="7">
-        <v>4</v>
-      </c>
-      <c r="J29" s="7">
-        <v>4</v>
-      </c>
-      <c r="K29" s="7"/>
-      <c r="L29" s="8"/>
+      <c r="B29" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="C29" s="9">
+        <v>2</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F29" s="9">
+        <v>2</v>
+      </c>
+      <c r="G29" s="9">
+        <v>2</v>
+      </c>
+      <c r="H29" s="9">
+        <v>1</v>
+      </c>
+      <c r="I29" s="9">
+        <v>0</v>
+      </c>
+      <c r="J29" s="9">
+        <v>0</v>
+      </c>
+      <c r="K29" s="9">
+        <v>0</v>
+      </c>
+      <c r="L29" s="9">
+        <v>0</v>
+      </c>
       <c r="M29" s="4"/>
       <c r="N29" s="4"/>
       <c r="O29" s="4"/>
@@ -2255,34 +2371,38 @@
     </row>
     <row r="30" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="9" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
       <c r="C30" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="D30" s="9" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="E30" s="9" t="s">
         <v>19</v>
       </c>
       <c r="F30" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G30" s="9">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H30" s="9">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I30" s="9">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="J30" s="9">
-        <v>0</v>
-      </c>
-      <c r="K30" s="9"/>
-      <c r="L30" s="9"/>
+        <v>3</v>
+      </c>
+      <c r="K30" s="9">
+        <v>1</v>
+      </c>
+      <c r="L30" s="9">
+        <v>1</v>
+      </c>
       <c r="M30" s="4"/>
       <c r="N30" s="4"/>
       <c r="O30" s="4"/>
@@ -2302,34 +2422,38 @@
     </row>
     <row r="31" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C31" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D31" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E31" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F31" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G31" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H31" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I31" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J31" s="9">
-        <v>3</v>
-      </c>
-      <c r="K31" s="9"/>
-      <c r="L31" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="K31" s="9">
+        <v>1</v>
+      </c>
+      <c r="L31" s="9">
+        <v>1</v>
+      </c>
       <c r="M31" s="4"/>
       <c r="N31" s="4"/>
       <c r="O31" s="4"/>
@@ -2347,82 +2471,90 @@
       <c r="AA31" s="4"/>
       <c r="AB31" s="4"/>
     </row>
-    <row r="32" spans="1:28" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B32" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C32" s="9">
-        <v>1</v>
-      </c>
-      <c r="D32" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E32" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F32" s="9">
-        <v>1</v>
-      </c>
-      <c r="G32" s="9">
-        <v>1</v>
-      </c>
-      <c r="H32" s="9">
-        <v>1</v>
-      </c>
-      <c r="I32" s="9">
-        <v>1</v>
-      </c>
-      <c r="J32" s="9">
-        <v>1</v>
-      </c>
-      <c r="K32" s="9"/>
-      <c r="L32" s="9"/>
-      <c r="M32" s="4"/>
-      <c r="N32" s="4"/>
-      <c r="O32" s="4"/>
-      <c r="P32" s="4"/>
-      <c r="Q32" s="4"/>
-      <c r="R32" s="4"/>
-      <c r="S32" s="4"/>
-      <c r="T32" s="4"/>
-      <c r="U32" s="4"/>
-      <c r="V32" s="4"/>
-      <c r="W32" s="4"/>
-      <c r="X32" s="4"/>
-      <c r="Y32" s="4"/>
-      <c r="Z32" s="4"/>
-      <c r="AA32" s="4"/>
-      <c r="AB32" s="4"/>
-    </row>
-    <row r="33" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="16"/>
-      <c r="B33" s="7" t="s">
+    <row r="32" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="16"/>
+      <c r="B32" s="7" t="s">
         <v>38</v>
       </c>
-      <c r="C33" s="7">
+      <c r="C32" s="7">
         <v>4</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D32" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="E33" s="8"/>
-      <c r="F33" s="7">
+      <c r="E32" s="8"/>
+      <c r="F32" s="7">
         <v>4</v>
       </c>
-      <c r="G33" s="7">
+      <c r="G32" s="7">
         <v>4</v>
       </c>
-      <c r="H33" s="7">
+      <c r="H32" s="7">
         <v>4</v>
       </c>
-      <c r="I33" s="7">
+      <c r="I32" s="7">
         <v>4</v>
       </c>
-      <c r="J33" s="7">
+      <c r="J32" s="7">
         <v>4</v>
       </c>
-      <c r="K33" s="7"/>
-      <c r="L33" s="8"/>
+      <c r="K32" s="7">
+        <v>3</v>
+      </c>
+      <c r="L32" s="7">
+        <v>3</v>
+      </c>
+      <c r="M32" s="11"/>
+      <c r="N32" s="11"/>
+      <c r="O32" s="11"/>
+      <c r="P32" s="11"/>
+      <c r="Q32" s="11"/>
+      <c r="R32" s="11"/>
+      <c r="S32" s="11"/>
+      <c r="T32" s="11"/>
+      <c r="U32" s="11"/>
+      <c r="V32" s="11"/>
+      <c r="W32" s="11"/>
+      <c r="X32" s="11"/>
+      <c r="Y32" s="11"/>
+      <c r="Z32" s="11"/>
+      <c r="AA32" s="11"/>
+      <c r="AB32" s="11"/>
+    </row>
+    <row r="33" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C33" s="9">
+        <v>3</v>
+      </c>
+      <c r="D33" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E33" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F33" s="9">
+        <v>3</v>
+      </c>
+      <c r="G33" s="9">
+        <v>3</v>
+      </c>
+      <c r="H33" s="9">
+        <v>3</v>
+      </c>
+      <c r="I33" s="9">
+        <v>3</v>
+      </c>
+      <c r="J33" s="9">
+        <v>3</v>
+      </c>
+      <c r="K33" s="9">
+        <v>1</v>
+      </c>
+      <c r="L33" s="9">
+        <v>1</v>
+      </c>
       <c r="M33" s="11"/>
       <c r="N33" s="11"/>
       <c r="O33" s="11"/>
@@ -2440,36 +2572,40 @@
       <c r="AA33" s="11"/>
       <c r="AB33" s="11"/>
     </row>
-    <row r="34" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C34" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D34" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E34" s="9" t="s">
         <v>25</v>
       </c>
       <c r="F34" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G34" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H34" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I34" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J34" s="9">
-        <v>3</v>
-      </c>
-      <c r="K34" s="9"/>
-      <c r="L34" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="K34" s="9">
+        <v>1</v>
+      </c>
+      <c r="L34" s="9">
+        <v>1</v>
+      </c>
       <c r="M34" s="11"/>
       <c r="N34" s="11"/>
       <c r="O34" s="11"/>
@@ -2487,36 +2623,38 @@
       <c r="AA34" s="11"/>
       <c r="AB34" s="11"/>
     </row>
-    <row r="35" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C35" s="9">
-        <v>1</v>
-      </c>
-      <c r="D35" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E35" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F35" s="9">
-        <v>1</v>
-      </c>
-      <c r="G35" s="9">
-        <v>1</v>
-      </c>
-      <c r="H35" s="9">
-        <v>1</v>
-      </c>
-      <c r="I35" s="9">
-        <v>1</v>
-      </c>
-      <c r="J35" s="9">
-        <v>1</v>
-      </c>
-      <c r="K35" s="9"/>
-      <c r="L35" s="9"/>
+    <row r="35" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B35" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C35" s="7">
+        <v>4</v>
+      </c>
+      <c r="D35" s="12" t="s">
+        <v>32</v>
+      </c>
+      <c r="E35" s="12"/>
+      <c r="F35" s="7">
+        <v>4</v>
+      </c>
+      <c r="G35" s="7">
+        <v>4</v>
+      </c>
+      <c r="H35" s="7">
+        <v>4</v>
+      </c>
+      <c r="I35" s="7">
+        <v>4</v>
+      </c>
+      <c r="J35" s="7">
+        <v>4</v>
+      </c>
+      <c r="K35" s="7">
+        <v>0</v>
+      </c>
+      <c r="L35" s="7">
+        <v>0</v>
+      </c>
       <c r="M35" s="11"/>
       <c r="N35" s="11"/>
       <c r="O35" s="11"/>
@@ -2534,34 +2672,40 @@
       <c r="AA35" s="11"/>
       <c r="AB35" s="11"/>
     </row>
-    <row r="36" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B36" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="C36" s="7">
-        <v>4</v>
-      </c>
-      <c r="D36" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="E36" s="12"/>
-      <c r="F36" s="7">
-        <v>4</v>
-      </c>
-      <c r="G36" s="7">
-        <v>4</v>
-      </c>
-      <c r="H36" s="7">
-        <v>4</v>
-      </c>
-      <c r="I36" s="7">
-        <v>4</v>
-      </c>
-      <c r="J36" s="7">
-        <v>4</v>
-      </c>
-      <c r="K36" s="7"/>
-      <c r="L36" s="8"/>
+    <row r="36" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B36" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C36" s="9">
+        <v>3</v>
+      </c>
+      <c r="D36" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E36" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F36" s="9">
+        <v>3</v>
+      </c>
+      <c r="G36" s="9">
+        <v>3</v>
+      </c>
+      <c r="H36" s="9">
+        <v>3</v>
+      </c>
+      <c r="I36" s="9">
+        <v>3</v>
+      </c>
+      <c r="J36" s="9">
+        <v>3</v>
+      </c>
+      <c r="K36" s="9">
+        <v>0</v>
+      </c>
+      <c r="L36" s="9">
+        <v>0</v>
+      </c>
       <c r="M36" s="11"/>
       <c r="N36" s="11"/>
       <c r="O36" s="11"/>
@@ -2579,36 +2723,40 @@
       <c r="AA36" s="11"/>
       <c r="AB36" s="11"/>
     </row>
-    <row r="37" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C37" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D37" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E37" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F37" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G37" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H37" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I37" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J37" s="9">
-        <v>3</v>
-      </c>
-      <c r="K37" s="9"/>
-      <c r="L37" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="K37" s="9">
+        <v>0</v>
+      </c>
+      <c r="L37" s="9">
+        <v>0</v>
+      </c>
       <c r="M37" s="11"/>
       <c r="N37" s="11"/>
       <c r="O37" s="11"/>
@@ -2626,36 +2774,38 @@
       <c r="AA37" s="11"/>
       <c r="AB37" s="11"/>
     </row>
-    <row r="38" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C38" s="9">
-        <v>1</v>
-      </c>
-      <c r="D38" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E38" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F38" s="9">
-        <v>1</v>
-      </c>
-      <c r="G38" s="9">
-        <v>1</v>
-      </c>
-      <c r="H38" s="9">
-        <v>1</v>
-      </c>
-      <c r="I38" s="9">
-        <v>1</v>
-      </c>
-      <c r="J38" s="9">
-        <v>1</v>
-      </c>
-      <c r="K38" s="9"/>
-      <c r="L38" s="9"/>
+    <row r="38" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B38" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="C38" s="7">
+        <v>4</v>
+      </c>
+      <c r="D38" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E38" s="12"/>
+      <c r="F38" s="7">
+        <v>4</v>
+      </c>
+      <c r="G38" s="7">
+        <v>4</v>
+      </c>
+      <c r="H38" s="7">
+        <v>4</v>
+      </c>
+      <c r="I38" s="7">
+        <v>4</v>
+      </c>
+      <c r="J38" s="7">
+        <v>3</v>
+      </c>
+      <c r="K38" s="7">
+        <v>2</v>
+      </c>
+      <c r="L38" s="7">
+        <v>2</v>
+      </c>
       <c r="M38" s="11"/>
       <c r="N38" s="11"/>
       <c r="O38" s="11"/>
@@ -2673,34 +2823,40 @@
       <c r="AA38" s="11"/>
       <c r="AB38" s="11"/>
     </row>
-    <row r="39" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B39" s="7" t="s">
-        <v>41</v>
-      </c>
-      <c r="C39" s="7">
-        <v>4</v>
-      </c>
-      <c r="D39" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="E39" s="12"/>
-      <c r="F39" s="7">
-        <v>4</v>
-      </c>
-      <c r="G39" s="7">
-        <v>4</v>
-      </c>
-      <c r="H39" s="7">
-        <v>4</v>
-      </c>
-      <c r="I39" s="7">
-        <v>4</v>
-      </c>
-      <c r="J39" s="7">
-        <v>3</v>
-      </c>
-      <c r="K39" s="7"/>
-      <c r="L39" s="8"/>
+    <row r="39" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B39" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C39" s="9">
+        <v>3</v>
+      </c>
+      <c r="D39" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E39" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F39" s="9">
+        <v>3</v>
+      </c>
+      <c r="G39" s="9">
+        <v>3</v>
+      </c>
+      <c r="H39" s="9">
+        <v>3</v>
+      </c>
+      <c r="I39" s="9">
+        <v>3</v>
+      </c>
+      <c r="J39" s="9">
+        <v>2</v>
+      </c>
+      <c r="K39" s="9">
+        <v>2</v>
+      </c>
+      <c r="L39" s="9">
+        <v>2</v>
+      </c>
       <c r="M39" s="11"/>
       <c r="N39" s="11"/>
       <c r="O39" s="11"/>
@@ -2718,36 +2874,40 @@
       <c r="AA39" s="11"/>
       <c r="AB39" s="11"/>
     </row>
-    <row r="40" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B40" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C40" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D40" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E40" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F40" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G40" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H40" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I40" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J40" s="9">
-        <v>2</v>
-      </c>
-      <c r="K40" s="9"/>
-      <c r="L40" s="9"/>
+        <v>1</v>
+      </c>
+      <c r="K40" s="9">
+        <v>0</v>
+      </c>
+      <c r="L40" s="9">
+        <v>0</v>
+      </c>
       <c r="M40" s="11"/>
       <c r="N40" s="11"/>
       <c r="O40" s="11"/>
@@ -2765,36 +2925,38 @@
       <c r="AA40" s="11"/>
       <c r="AB40" s="11"/>
     </row>
-    <row r="41" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C41" s="9">
-        <v>1</v>
-      </c>
-      <c r="D41" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E41" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F41" s="9">
-        <v>1</v>
-      </c>
-      <c r="G41" s="9">
-        <v>1</v>
-      </c>
-      <c r="H41" s="9">
-        <v>1</v>
-      </c>
-      <c r="I41" s="9">
-        <v>1</v>
-      </c>
-      <c r="J41" s="9">
-        <v>1</v>
-      </c>
-      <c r="K41" s="9"/>
-      <c r="L41" s="9"/>
+    <row r="41" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B41" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="C41" s="7">
+        <v>4</v>
+      </c>
+      <c r="D41" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E41" s="12"/>
+      <c r="F41" s="7">
+        <v>4</v>
+      </c>
+      <c r="G41" s="17">
+        <v>4</v>
+      </c>
+      <c r="H41" s="17">
+        <v>4</v>
+      </c>
+      <c r="I41" s="17">
+        <v>4</v>
+      </c>
+      <c r="J41" s="17">
+        <v>2</v>
+      </c>
+      <c r="K41" s="17">
+        <v>0</v>
+      </c>
+      <c r="L41" s="17">
+        <v>0</v>
+      </c>
       <c r="M41" s="11"/>
       <c r="N41" s="11"/>
       <c r="O41" s="11"/>
@@ -2812,34 +2974,40 @@
       <c r="AA41" s="11"/>
       <c r="AB41" s="11"/>
     </row>
-    <row r="42" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B42" s="14" t="s">
-        <v>43</v>
-      </c>
-      <c r="C42" s="7">
-        <v>4</v>
-      </c>
-      <c r="D42" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E42" s="12"/>
-      <c r="F42" s="7">
-        <v>4</v>
-      </c>
-      <c r="G42" s="17">
-        <v>4</v>
-      </c>
-      <c r="H42" s="17">
-        <v>4</v>
-      </c>
-      <c r="I42" s="17">
-        <v>4</v>
-      </c>
-      <c r="J42" s="17">
+    <row r="42" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B42" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C42" s="9">
+        <v>3</v>
+      </c>
+      <c r="D42" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E42" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="F42" s="9">
+        <v>3</v>
+      </c>
+      <c r="G42" s="9">
+        <v>3</v>
+      </c>
+      <c r="H42" s="9">
+        <v>3</v>
+      </c>
+      <c r="I42" s="9">
+        <v>3</v>
+      </c>
+      <c r="J42" s="9">
         <v>2</v>
       </c>
-      <c r="K42" s="14"/>
-      <c r="L42" s="12"/>
+      <c r="K42" s="9">
+        <v>0</v>
+      </c>
+      <c r="L42" s="9">
+        <v>0</v>
+      </c>
       <c r="M42" s="11"/>
       <c r="N42" s="11"/>
       <c r="O42" s="11"/>
@@ -2857,36 +3025,40 @@
       <c r="AA42" s="11"/>
       <c r="AB42" s="11"/>
     </row>
-    <row r="43" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B43" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C43" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D43" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E43" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F43" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G43" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H43" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I43" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="J43" s="9">
-        <v>2</v>
-      </c>
-      <c r="K43" s="9"/>
-      <c r="L43" s="9"/>
+        <v>0</v>
+      </c>
+      <c r="K43" s="9">
+        <v>0</v>
+      </c>
+      <c r="L43" s="9">
+        <v>0</v>
+      </c>
       <c r="M43" s="11"/>
       <c r="N43" s="11"/>
       <c r="O43" s="11"/>
@@ -2904,36 +3076,38 @@
       <c r="AA43" s="11"/>
       <c r="AB43" s="11"/>
     </row>
-    <row r="44" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C44" s="9">
-        <v>1</v>
-      </c>
-      <c r="D44" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E44" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F44" s="9">
-        <v>1</v>
-      </c>
-      <c r="G44" s="9">
-        <v>1</v>
-      </c>
-      <c r="H44" s="9">
-        <v>1</v>
-      </c>
-      <c r="I44" s="9">
-        <v>1</v>
-      </c>
-      <c r="J44" s="9">
-        <v>0</v>
-      </c>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
+    <row r="44" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B44" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="C44" s="7">
+        <v>4</v>
+      </c>
+      <c r="D44" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" s="12"/>
+      <c r="F44" s="7">
+        <v>4</v>
+      </c>
+      <c r="G44" s="17">
+        <v>4</v>
+      </c>
+      <c r="H44" s="17">
+        <v>4</v>
+      </c>
+      <c r="I44" s="17">
+        <v>3</v>
+      </c>
+      <c r="J44" s="17">
+        <v>1.5</v>
+      </c>
+      <c r="K44" s="17">
+        <v>1</v>
+      </c>
+      <c r="L44" s="17">
+        <v>1</v>
+      </c>
       <c r="M44" s="11"/>
       <c r="N44" s="11"/>
       <c r="O44" s="11"/>
@@ -2951,34 +3125,40 @@
       <c r="AA44" s="11"/>
       <c r="AB44" s="11"/>
     </row>
-    <row r="45" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="C45" s="7">
-        <v>4</v>
-      </c>
-      <c r="D45" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="E45" s="12"/>
-      <c r="F45" s="7">
-        <v>4</v>
-      </c>
-      <c r="G45" s="17">
-        <v>4</v>
-      </c>
-      <c r="H45" s="17">
-        <v>4</v>
-      </c>
-      <c r="I45" s="17">
-        <v>3</v>
-      </c>
-      <c r="J45" s="17">
-        <v>1.5</v>
-      </c>
-      <c r="K45" s="14"/>
-      <c r="L45" s="12"/>
+    <row r="45" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C45" s="9">
+        <v>3</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="E45" s="9" t="s">
+        <v>19</v>
+      </c>
+      <c r="F45" s="9">
+        <v>3</v>
+      </c>
+      <c r="G45" s="9">
+        <v>3</v>
+      </c>
+      <c r="H45" s="9">
+        <v>3</v>
+      </c>
+      <c r="I45" s="9">
+        <v>2</v>
+      </c>
+      <c r="J45" s="9">
+        <v>1</v>
+      </c>
+      <c r="K45" s="9">
+        <v>1</v>
+      </c>
+      <c r="L45" s="9">
+        <v>1</v>
+      </c>
       <c r="M45" s="11"/>
       <c r="N45" s="11"/>
       <c r="O45" s="11"/>
@@ -2996,36 +3176,40 @@
       <c r="AA45" s="11"/>
       <c r="AB45" s="11"/>
     </row>
-    <row r="46" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="9" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="C46" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="D46" s="9" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="E46" s="9" t="s">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="F46" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G46" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="H46" s="9">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I46" s="9">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="J46" s="9">
-        <v>1</v>
-      </c>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
+        <v>0.5</v>
+      </c>
+      <c r="K46" s="9">
+        <v>0</v>
+      </c>
+      <c r="L46" s="9">
+        <v>0</v>
+      </c>
       <c r="M46" s="11"/>
       <c r="N46" s="11"/>
       <c r="O46" s="11"/>
@@ -3043,85 +3227,66 @@
       <c r="AA46" s="11"/>
       <c r="AB46" s="11"/>
     </row>
-    <row r="47" spans="1:28" s="10" customFormat="1" ht="25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B47" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="C47" s="9">
-        <v>1</v>
-      </c>
-      <c r="D47" s="9" t="s">
-        <v>27</v>
-      </c>
-      <c r="E47" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="F47" s="9">
-        <v>1</v>
-      </c>
-      <c r="G47" s="9">
-        <v>1</v>
-      </c>
-      <c r="H47" s="9">
-        <v>1</v>
-      </c>
-      <c r="I47" s="9">
-        <v>1</v>
-      </c>
-      <c r="J47" s="9">
-        <v>0.5</v>
-      </c>
-      <c r="K47" s="9"/>
-      <c r="L47" s="9"/>
-      <c r="M47" s="11"/>
-      <c r="N47" s="11"/>
-      <c r="O47" s="11"/>
-      <c r="P47" s="11"/>
-      <c r="Q47" s="11"/>
-      <c r="R47" s="11"/>
-      <c r="S47" s="11"/>
-      <c r="T47" s="11"/>
-      <c r="U47" s="11"/>
-      <c r="V47" s="11"/>
-      <c r="W47" s="11"/>
-      <c r="X47" s="11"/>
-      <c r="Y47" s="11"/>
-      <c r="Z47" s="11"/>
-      <c r="AA47" s="11"/>
-      <c r="AB47" s="11"/>
-    </row>
-    <row r="48" spans="1:28" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B48" s="5" t="s">
+    <row r="47" spans="2:28" ht="35.15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B47" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="C48" s="5">
+      <c r="C47" s="5">
         <v>68</v>
       </c>
-      <c r="D48" s="5"/>
-      <c r="E48" s="5"/>
-      <c r="F48" s="5">
-        <f>F45+F42+F39+F36+F33+F29+F24+F20+F17+F13+F9+F7+F5+F3</f>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5">
+        <f>F44+F41+F38+F35+F32+F28+F24+F20+F17+F13+F9+F7+F5+F3</f>
         <v>68</v>
       </c>
-      <c r="G48" s="5">
+      <c r="G47" s="5">
         <v>63</v>
       </c>
-      <c r="H48" s="5">
+      <c r="H47" s="5">
         <v>53</v>
       </c>
-      <c r="I48" s="5">
+      <c r="I47" s="5">
         <v>44</v>
       </c>
-      <c r="J48" s="5">
+      <c r="J47" s="5">
         <v>34.5</v>
       </c>
-      <c r="K48" s="5">
-        <v>0</v>
-      </c>
-      <c r="L48" s="5">
-        <f>SUM(L3:L33)</f>
-        <v>0</v>
-      </c>
+      <c r="K47" s="5">
+        <v>17</v>
+      </c>
+      <c r="L47" s="5">
+        <v>17</v>
+      </c>
+      <c r="M47" s="4"/>
+      <c r="N47" s="4"/>
+      <c r="O47" s="4"/>
+      <c r="P47" s="4"/>
+      <c r="Q47" s="4"/>
+      <c r="R47" s="4"/>
+      <c r="S47" s="4"/>
+      <c r="T47" s="4"/>
+      <c r="U47" s="4"/>
+      <c r="V47" s="4"/>
+      <c r="W47" s="4"/>
+      <c r="X47" s="4"/>
+      <c r="Y47" s="4"/>
+      <c r="Z47" s="4"/>
+      <c r="AA47" s="4"/>
+      <c r="AB47" s="4"/>
+    </row>
+    <row r="48" spans="2:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B48" s="4"/>
+      <c r="C48" s="1"/>
+      <c r="D48" s="4"/>
+      <c r="E48" s="4"/>
+      <c r="F48" s="4"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+      <c r="J48" s="4"/>
+      <c r="K48" s="4"/>
+      <c r="L48" s="4"/>
       <c r="M48" s="4"/>
       <c r="N48" s="4"/>
       <c r="O48" s="4"/>
@@ -3139,28 +3304,28 @@
       <c r="AA48" s="4"/>
       <c r="AB48" s="4"/>
     </row>
-    <row r="49" spans="2:28" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="4"/>
-      <c r="C49" s="1"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
-      <c r="H49" s="4"/>
-      <c r="I49" s="4"/>
-      <c r="J49" s="4"/>
-      <c r="K49" s="4"/>
-      <c r="L49" s="4"/>
-      <c r="M49" s="4"/>
-      <c r="N49" s="4"/>
-      <c r="O49" s="4"/>
-      <c r="P49" s="4"/>
-      <c r="Q49" s="4"/>
-      <c r="R49" s="4"/>
-      <c r="S49" s="4"/>
-      <c r="T49" s="4"/>
-      <c r="U49" s="4"/>
-      <c r="V49" s="4"/>
+    <row r="49" spans="2:28" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="20"/>
+      <c r="C49" s="20"/>
+      <c r="D49" s="20"/>
+      <c r="E49" s="20"/>
+      <c r="F49" s="20"/>
+      <c r="G49" s="20"/>
+      <c r="H49" s="20"/>
+      <c r="I49" s="20"/>
+      <c r="J49" s="20"/>
+      <c r="K49" s="20"/>
+      <c r="L49" s="20"/>
+      <c r="M49" s="20"/>
+      <c r="N49" s="20"/>
+      <c r="O49" s="20"/>
+      <c r="P49" s="20"/>
+      <c r="Q49" s="20"/>
+      <c r="R49" s="20"/>
+      <c r="S49" s="20"/>
+      <c r="T49" s="20"/>
+      <c r="U49" s="20"/>
+      <c r="V49" s="20"/>
       <c r="W49" s="4"/>
       <c r="X49" s="4"/>
       <c r="Y49" s="4"/>
@@ -3168,28 +3333,28 @@
       <c r="AA49" s="4"/>
       <c r="AB49" s="4"/>
     </row>
-    <row r="50" spans="2:28" ht="50.15" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="B50" s="19"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="19"/>
-      <c r="E50" s="19"/>
-      <c r="F50" s="19"/>
-      <c r="G50" s="19"/>
-      <c r="H50" s="19"/>
-      <c r="I50" s="19"/>
-      <c r="J50" s="19"/>
-      <c r="K50" s="19"/>
-      <c r="L50" s="19"/>
-      <c r="M50" s="19"/>
-      <c r="N50" s="19"/>
-      <c r="O50" s="19"/>
-      <c r="P50" s="19"/>
-      <c r="Q50" s="19"/>
-      <c r="R50" s="19"/>
-      <c r="S50" s="19"/>
-      <c r="T50" s="19"/>
-      <c r="U50" s="19"/>
-      <c r="V50" s="19"/>
+    <row r="50" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B50" s="4"/>
+      <c r="C50" s="1"/>
+      <c r="D50" s="4"/>
+      <c r="E50" s="4"/>
+      <c r="F50" s="4"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+      <c r="J50" s="4"/>
+      <c r="K50" s="4"/>
+      <c r="L50" s="4"/>
+      <c r="M50" s="4"/>
+      <c r="N50" s="4"/>
+      <c r="O50" s="4"/>
+      <c r="P50" s="4"/>
+      <c r="Q50" s="4"/>
+      <c r="R50" s="4"/>
+      <c r="S50" s="4"/>
+      <c r="T50" s="4"/>
+      <c r="U50" s="4"/>
+      <c r="V50" s="4"/>
       <c r="W50" s="4"/>
       <c r="X50" s="4"/>
       <c r="Y50" s="4"/>
@@ -3260,7 +3425,7 @@
       <c r="C53" s="1"/>
       <c r="D53" s="4"/>
       <c r="E53" s="4"/>
-      <c r="F53" s="4"/>
+      <c r="F53" s="15"/>
       <c r="G53" s="4"/>
       <c r="H53" s="4"/>
       <c r="I53" s="4"/>
@@ -3289,7 +3454,7 @@
       <c r="C54" s="1"/>
       <c r="D54" s="4"/>
       <c r="E54" s="4"/>
-      <c r="F54" s="15"/>
+      <c r="F54" s="4"/>
       <c r="G54" s="4"/>
       <c r="H54" s="4"/>
       <c r="I54" s="4"/>
@@ -5894,42 +6059,13 @@
       <c r="AA143" s="4"/>
       <c r="AB143" s="4"/>
     </row>
-    <row r="144" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B144" s="4"/>
-      <c r="C144" s="1"/>
-      <c r="D144" s="4"/>
-      <c r="E144" s="4"/>
-      <c r="F144" s="4"/>
-      <c r="G144" s="4"/>
-      <c r="H144" s="4"/>
-      <c r="I144" s="4"/>
-      <c r="J144" s="4"/>
-      <c r="K144" s="4"/>
-      <c r="L144" s="4"/>
-      <c r="M144" s="4"/>
-      <c r="N144" s="4"/>
-      <c r="O144" s="4"/>
-      <c r="P144" s="4"/>
-      <c r="Q144" s="4"/>
-      <c r="R144" s="4"/>
-      <c r="S144" s="4"/>
-      <c r="T144" s="4"/>
-      <c r="U144" s="4"/>
-      <c r="V144" s="4"/>
-      <c r="W144" s="4"/>
-      <c r="X144" s="4"/>
-      <c r="Y144" s="4"/>
-      <c r="Z144" s="4"/>
-      <c r="AA144" s="4"/>
-      <c r="AB144" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:V1"/>
-    <mergeCell ref="B50:V50"/>
+    <mergeCell ref="B49:V49"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E43:E44 E46:E47 E3:E41" xr:uid="{0ECFFA54-49B0-4052-A5A6-9F9B9CD7A0FF}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E42:E43 E45:E46 E3:E40" xr:uid="{0ECFFA54-49B0-4052-A5A6-9F9B9CD7A0FF}">
       <formula1>"Not Started, In Progress, Completed"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>